<commit_message>
aktualizacja parametrow i rysunkow
</commit_message>
<xml_diff>
--- a/parametry.xlsx
+++ b/parametry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BT\Documents\GitHub\ProjektyDCN\01_Studnie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://texoanalytics-my.sharepoint.com/personal/bz_texo-analytics_com/Documents/Documents/GitHub/ProjektyDCN/01_Studnie/v1. pliki źródłowe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2183EA0-0704-4EBC-8D6D-C725E1B0F827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="13_ncr:1_{E9F97993-CD50-45C4-BEA2-EDE3877E0362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{794CCEF4-0BD3-47FE-AD28-12E6E842B3BC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studnie" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="124">
   <si>
     <t>Property Type</t>
   </si>
@@ -284,62 +283,148 @@
     <t>Jednostki</t>
   </si>
   <si>
-    <t>Wartość</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>ID studnia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otwór </t>
-  </si>
-  <si>
-    <t>o-1</t>
-  </si>
-  <si>
-    <t>Typ</t>
-  </si>
-  <si>
-    <t>stud-1</t>
-  </si>
-  <si>
-    <t>stud-2</t>
-  </si>
-  <si>
-    <t>stud-3</t>
-  </si>
-  <si>
-    <t>o-1,o-2</t>
-  </si>
-  <si>
-    <t>o-1,o-2,o-3</t>
-  </si>
-  <si>
-    <t>Openings</t>
-  </si>
-  <si>
-    <t>Chamber ID</t>
-  </si>
-  <si>
-    <t>dopływ</t>
-  </si>
-  <si>
-    <t>o-2</t>
-  </si>
-  <si>
-    <t>o-3</t>
-  </si>
-  <si>
-    <t>wylot</t>
+    <t>STUD-1</t>
+  </si>
+  <si>
+    <t>STUD-2</t>
+  </si>
+  <si>
+    <t>STUD-4</t>
+  </si>
+  <si>
+    <t>STUD-3</t>
+  </si>
+  <si>
+    <t>STUD-5</t>
+  </si>
+  <si>
+    <t>WYLOT-1</t>
+  </si>
+  <si>
+    <t>WYLOT-2</t>
+  </si>
+  <si>
+    <t>WYLOT-3</t>
+  </si>
+  <si>
+    <t>Przykładowa Wartość</t>
+  </si>
+  <si>
+    <t>concrete</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>flat</t>
+  </si>
+  <si>
+    <t>seal</t>
+  </si>
+  <si>
+    <t>coated</t>
+  </si>
+  <si>
+    <t>flase</t>
+  </si>
+  <si>
+    <t>C35/45</t>
+  </si>
+  <si>
+    <t>IDStudni</t>
+  </si>
+  <si>
+    <t>KlasaSN</t>
+  </si>
+  <si>
+    <t>Parametry otworów  bazujące na IfcPort</t>
+  </si>
+  <si>
+    <t>FlowDirection</t>
+  </si>
+  <si>
+    <t>Enumeration that identifies if this port is a Sink (inlet), a Source (outlet) or both a SinkAndSource.</t>
+  </si>
+  <si>
+    <t>PortNumber</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>The Diameter of the object</t>
+  </si>
+  <si>
+    <t>średnica rury</t>
+  </si>
+  <si>
+    <t>DistanceToInvertLevel</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>IfcPositiveDegreeMeasure</t>
+  </si>
+  <si>
+    <t>ActualPortDiameter</t>
+  </si>
+  <si>
+    <t>2,4,8</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>Rzeczywista średnica otworu</t>
+  </si>
+  <si>
+    <t>Numer otworu indywidualny dla studni</t>
+  </si>
+  <si>
+    <t>Indywidualny identyfikator opisywanej studni</t>
+  </si>
+  <si>
+    <t>SINK = wlot
+SOURCE = wylot</t>
+  </si>
+  <si>
+    <t>SINK
+SOURCE</t>
+  </si>
+  <si>
+    <t>lekkia (SN = 2 kPa), DN 110–400 mm,
+średnia (SN = 4 kPa ), DN 110–400 mm,
+ciężka (SN = 8 kPa), DN 110–400 mm.</t>
+  </si>
+  <si>
+    <t>Indywidualny identyfikator opisywanej studni. 
+Nawet jeśli studnie sa identyczne to powinny mieć indywidualne identyfikatory</t>
+  </si>
+  <si>
+    <t>Odległość od dna studni do osi otworu</t>
+  </si>
+  <si>
+    <t>Kąt osi otworu mierzon od osi mierzony od wylotu (wylot =0)</t>
+  </si>
+  <si>
+    <t>ZESTAWIENIE OTWORÓW</t>
+  </si>
+  <si>
+    <t>ZESTAWIENIE STUDNI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,8 +483,37 @@
       <name val="Open Sans"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Open Sans"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Open Sans"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +532,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -471,14 +597,123 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color auto="1"/>
       </left>
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -486,7 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -499,15 +734,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -519,9 +745,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -531,34 +754,99 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -567,6 +855,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDEBF7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -623,6 +916,204 @@
         <a:xfrm>
           <a:off x="12604750" y="1730375"/>
           <a:ext cx="2876550" cy="1138970"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2753473</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>115048</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{530B026B-ADFA-48F3-8EC8-678EFC8F6718}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13567149" y="89647"/>
+          <a:ext cx="2752725" cy="1145133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1143928</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{618B9CEF-6D51-403E-BDAA-235C61863E2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="527538" y="0"/>
+          <a:ext cx="1114621" cy="473075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>252291</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>506487</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C183F56-69B9-4C0B-BEE4-A14ADA0E4B81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="252291" y="0"/>
+          <a:ext cx="1114621" cy="469900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -912,481 +1403,515 @@
   </sheetPr>
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="27.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="49.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="27.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="1" customWidth="1"/>
+    <col min="6" max="7" width="49.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33.1796875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="21" t="s">
         <v>74</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F6" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <v>3000</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="13">
+        <v>-3.5</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="13">
+        <v>-1</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="13">
+        <v>150</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10" t="s">
+      <c r="D16" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="13">
+        <v>200</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:7" ht="62" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10" t="s">
+      <c r="D19" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="13">
+        <v>600</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10" t="s">
+      <c r="D21" s="13"/>
+      <c r="E21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="10" t="s">
+      <c r="D22" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="14">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="10" t="s">
+      <c r="F23" s="6"/>
+      <c r="G23" s="27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="10" t="s">
+      <c r="D24" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10" t="s">
+      <c r="F24" s="6"/>
+      <c r="G24" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="10" t="s">
+      <c r="D25" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="10" t="s">
+      <c r="F25" s="11"/>
+      <c r="G25" s="27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="10" t="s">
+      <c r="D26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="10" t="s">
+      <c r="F26" s="11"/>
+      <c r="G26" s="27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="10" t="s">
+      <c r="D27" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="10" t="s">
+      <c r="F27" s="11"/>
+      <c r="G27" s="27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+    <row r="28" spans="1:7" ht="46.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="10" t="s">
+      <c r="D28" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>91</v>
-      </c>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E29" s="2"/>
       <c r="G29" s="2"/>
     </row>
@@ -1396,349 +1921,610 @@
     <hyperlink ref="F2" r:id="rId1" xr:uid="{6183636E-2633-40A0-94B1-C7692C3F5647}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" verticalDpi="4294967293" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2714233-993F-4C9B-8B24-C807A312DF25}">
-  <dimension ref="A2:B10"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.1796875" customWidth="1"/>
+    <col min="7" max="7" width="37.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>19</v>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A10" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1" display="https://search.bsdd.buildingsmart.org/ClassificationProperty/Index/454277" xr:uid="{5D5EDC57-6896-4882-8EE2-2D3BEDAA57EE}"/>
+    <hyperlink ref="A12" r:id="rId2" display="https://search.bsdd.buildingsmart.org/Property/Index/116738" xr:uid="{2921D386-C856-46AC-8B9D-F8ACB0E49652}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F3BEAF-4C70-4BDF-990B-EC7D211C6D39}">
-  <dimension ref="A1:U4"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="18"/>
-    <col min="4" max="4" width="11.140625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="18" customWidth="1"/>
-    <col min="9" max="12" width="9.140625" style="18"/>
-    <col min="13" max="13" width="7.7109375" style="18" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="18" customWidth="1"/>
-    <col min="15" max="16" width="10.140625" style="18" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="18"/>
-    <col min="18" max="18" width="7.28515625" style="18" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="18" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="18"/>
-    <col min="21" max="21" width="10.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" s="24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="U3" s="26" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+    </row>
+    <row r="6" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+    </row>
+    <row r="7" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="U4" s="26" t="s">
-        <v>89</v>
-      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+    </row>
+    <row r="8" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+    </row>
+    <row r="9" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83898226-07C1-40D8-A0B0-3EBB9154117C}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="https://search.bsdd.buildingsmart.org/ClassificationProperty/Index/454277" xr:uid="{4C5D544B-6F57-4FBC-A383-3BD5FC77DFD4}"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://search.bsdd.buildingsmart.org/Property/Index/116738" xr:uid="{E24586D6-139B-41AA-9385-5EBFE7FB6C5D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>